<commit_message>
agregando el modulo de runner_excel.py para tener un codigo mas limpio y escalable
</commit_message>
<xml_diff>
--- a/Manejar_Excel/datos.xlsx
+++ b/Manejar_Excel/datos.xlsx
@@ -390,7 +390,7 @@
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>insterado</t>
+          <t>insertado</t>
         </is>
       </c>
       <c r="F2" s="2" t="n"/>
@@ -418,7 +418,7 @@
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>insterado</t>
+          <t>insertado</t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>insterado</t>
+          <t>insertado</t>
         </is>
       </c>
       <c r="F4" s="2" t="n"/>
@@ -474,7 +474,7 @@
       </c>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>insterado</t>
+          <t>insertado</t>
         </is>
       </c>
       <c r="F5" s="2" t="n"/>

</xml_diff>